<commit_message>
Mise à jour du 02.06.2017
Gros ajout sur la documentation, et finition du programme
</commit_message>
<xml_diff>
--- a/Documentation/X-TPI-pittierst-GrilleDeTests.xlsx
+++ b/Documentation/X-TPI-pittierst-GrilleDeTests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>Fonction à tester</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Le massageBox s'affiche bien et permet de montrer les informations de bases</t>
+  </si>
+  <si>
+    <t>La fonction fonctionne mais il reste un petit soucis. Quand je multiplie une valeur 2 plus grande que la valeur 1 le code plante</t>
+  </si>
+  <si>
+    <t>Le programme affiche le résultat</t>
   </si>
 </sst>
 </file>
@@ -275,12 +281,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -289,6 +289,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,10 +579,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +592,7 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -608,20 +614,20 @@
       <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -630,10 +636,10 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -649,10 +655,10 @@
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -668,10 +674,10 @@
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -687,10 +693,10 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -706,10 +712,10 @@
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -727,10 +733,10 @@
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -746,10 +752,10 @@
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -765,10 +771,10 @@
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="8">
-        <v>42887</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -784,8 +790,8 @@
       <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8">
-        <v>42522</v>
+      <c r="C11" s="6">
+        <v>42887</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>41</v>
@@ -805,7 +811,7 @@
       <c r="B12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>42887</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -818,15 +824,15 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -835,8 +841,8 @@
       <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8">
-        <v>42522</v>
+      <c r="C14" s="6">
+        <v>42887</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>37</v>
@@ -854,8 +860,8 @@
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="8">
-        <v>42522</v>
+      <c r="C15" s="6">
+        <v>42887</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>37</v>
@@ -873,8 +879,8 @@
       <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="8">
-        <v>42522</v>
+      <c r="C16" s="6">
+        <v>42887</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -894,8 +900,8 @@
       <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="8">
-        <v>42522</v>
+      <c r="C17" s="6">
+        <v>42887</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>37</v>
@@ -915,8 +921,8 @@
       <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="8">
-        <v>42522</v>
+      <c r="C18" s="6">
+        <v>42887</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>41</v>
@@ -933,55 +939,55 @@
     </row>
     <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="8">
-        <v>42522</v>
+      <c r="C19" s="6">
+        <v>42888</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="8">
-        <v>42522</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="8">
-        <v>42522</v>
+      <c r="C21" s="6">
+        <v>42887</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>37</v>
@@ -994,36 +1000,36 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="8">
-        <v>42522</v>
+        <v>29</v>
+      </c>
+      <c r="C22" s="6">
+        <v>42887</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="8">
-        <v>42522</v>
+      <c r="C23" s="6">
+        <v>42887</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>41</v>
@@ -1038,13 +1044,13 @@
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="8">
-        <v>42522</v>
+      <c r="C24" s="6">
+        <v>42887</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>41</v>
@@ -1057,14 +1063,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="1"/>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="6">
+        <v>42887</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1130,8 +1148,8 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1290,6 +1308,15 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>